<commit_message>
finalizing nvessels script + small xlsx fix
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb159/raw/Table5.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb159/raw/Table5.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/fb159/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb159/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AFC539-A198-5B41-9787-0A2CB9E3864C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2DE41C-68AA-AD47-949E-F7137E37A887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="4420" windowWidth="27640" windowHeight="16940" xr2:uid="{6D70A715-AA2C-B24D-AB74-433D8CD08086}"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" xr2:uid="{6D70A715-AA2C-B24D-AB74-433D8CD08086}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -102,9 +110,6 @@
     <t>101-105</t>
   </si>
   <si>
-    <t>100-110</t>
-  </si>
-  <si>
     <t>111-115</t>
   </si>
   <si>
@@ -129,25 +134,28 @@
     <t>146-150</t>
   </si>
   <si>
-    <t>150-160</t>
-  </si>
-  <si>
     <t>161-165</t>
   </si>
   <si>
-    <t>160-170</t>
-  </si>
-  <si>
     <t>171-175</t>
   </si>
   <si>
-    <t>170-180,</t>
-  </si>
-  <si>
     <t>151-155</t>
   </si>
   <si>
     <t>11-15</t>
+  </si>
+  <si>
+    <t>106-110</t>
+  </si>
+  <si>
+    <t>166-170</t>
+  </si>
+  <si>
+    <t>176-180,</t>
+  </si>
+  <si>
+    <t>156-160</t>
   </si>
 </sst>
 </file>
@@ -512,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C845E-3A65-1A4E-9E1D-D14B19AAEA7D}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +557,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>125</v>
@@ -758,7 +766,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -769,7 +777,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -780,7 +788,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -791,7 +799,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -802,7 +810,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>12</v>
@@ -813,7 +821,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>11</v>
@@ -824,7 +832,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>11</v>
@@ -835,7 +843,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -846,7 +854,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -857,7 +865,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>11</v>
@@ -868,7 +876,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -879,7 +887,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -890,7 +898,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -901,7 +909,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -912,7 +920,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>0</v>

</xml_diff>